<commit_message>
Restored 'Zeitaufzeichnung' to its previous state. (Table Tobias W.
</commit_message>
<xml_diff>
--- a/05_Zeitaufzeichnung/Zeitaufzeichnung_Local_Admin.xlsx
+++ b/05_Zeitaufzeichnung/Zeitaufzeichnung_Local_Admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nils\Desktop\Schule\ITP\Local Admin\05_Zeitaufzeichnung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITP\LocalAdmin\project-management\05_Zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF28961-D2AF-4CB8-8AC6-8F4F696E398E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321A499E-656F-448E-9887-5681BE29471C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="13770" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allg." sheetId="1" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
   <si>
     <t>Aktivität</t>
   </si>
@@ -269,6 +271,15 @@
   </si>
   <si>
     <t>Datenstruktur in worte fassen</t>
+  </si>
+  <si>
+    <t>18.10.2019</t>
+  </si>
+  <si>
+    <t>Nutzwertanalyse - Lizenzserver</t>
+  </si>
+  <si>
+    <t>Nutzwertanalyse - Datenformate</t>
   </si>
 </sst>
 </file>
@@ -659,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -913,6 +924,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2416,7 +2434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42714C1D-C593-464A-80BF-C213BA577893}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
@@ -3297,6 +3315,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A26:A46"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B46"/>
     <mergeCell ref="A2:A22"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B8"/>
@@ -3304,13 +3329,6 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A26:A46"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3318,10 +3336,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4C5F66-E89D-4EAB-B57A-C68CB0901AD5}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3366,10 +3384,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="119" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="105" t="s">
@@ -3396,8 +3414,8 @@
       <c r="J2" s="106"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="136"/>
+      <c r="A3" s="132"/>
+      <c r="B3" s="120"/>
       <c r="C3" s="105" t="s">
         <v>62</v>
       </c>
@@ -3422,8 +3440,8 @@
       <c r="J3" s="106"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="139"/>
-      <c r="B4" s="136"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="120"/>
       <c r="C4" s="105" t="s">
         <v>63</v>
       </c>
@@ -3448,8 +3466,8 @@
       <c r="J4" s="106"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="139"/>
-      <c r="B5" s="136"/>
+      <c r="A5" s="132"/>
+      <c r="B5" s="120"/>
       <c r="C5" s="105" t="s">
         <v>63</v>
       </c>
@@ -3468,8 +3486,8 @@
       <c r="J5" s="106"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="139"/>
-      <c r="B6" s="136"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="120"/>
       <c r="C6" s="105" t="s">
         <v>68</v>
       </c>
@@ -3494,114 +3512,120 @@
       <c r="J6" s="106"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="139"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="107">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F7" s="107">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="G7" s="106"/>
       <c r="H7" s="106"/>
       <c r="I7" s="106"/>
       <c r="J7" s="106"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="139"/>
-      <c r="B8" s="138" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="105" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="106" t="s">
-        <v>34</v>
+      <c r="A8" s="132"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="141" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="142" t="s">
+        <v>78</v>
       </c>
       <c r="E8" s="107">
-        <v>0.55555555555555558</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="107">
-        <v>0.63194444444444442</v>
-      </c>
-      <c r="G8" s="107">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H8" s="107">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="I8" s="107">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="J8" s="106"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="139"/>
-      <c r="B9" s="139"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="141" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="107">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F9" s="107">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="G9" s="106"/>
       <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="139"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="106"/>
+      <c r="A10" s="132"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="142"/>
       <c r="E10" s="106"/>
       <c r="F10" s="106"/>
       <c r="G10" s="106"/>
       <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="106"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="137"/>
+      <c r="A11" s="132"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="105"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="106" t="s">
-        <v>65</v>
+      <c r="A12" s="132"/>
+      <c r="B12" s="138" t="s">
+        <v>64</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="D12" s="106" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="107">
-        <v>0.70833333333333337</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F12" s="107">
-        <v>0.79166666666666663</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="G12" s="107">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H12" s="107">
-        <v>8.3333333333333329E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
       <c r="I12" s="107">
-        <v>4.1666666666666664E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="J12" s="106"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="136"/>
-      <c r="B13" s="105"/>
+      <c r="A13" s="132"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="105"/>
       <c r="D13" s="106"/>
       <c r="E13" s="106"/>
@@ -3612,8 +3636,8 @@
       <c r="J13" s="106"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="136"/>
-      <c r="B14" s="105"/>
+      <c r="A14" s="132"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="105"/>
       <c r="D14" s="106"/>
       <c r="E14" s="106"/>
@@ -3624,8 +3648,8 @@
       <c r="J14" s="106"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="136"/>
-      <c r="B15" s="105"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="137"/>
       <c r="C15" s="105"/>
       <c r="D15" s="106"/>
       <c r="E15" s="106"/>
@@ -3635,13 +3659,79 @@
       <c r="I15" s="106"/>
       <c r="J15" s="106"/>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="138" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="106" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="106" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="107">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F16" s="107">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G16" s="107">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H16" s="107">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I16" s="107">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J16" s="106"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="139"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="139"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="137"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A2:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>